<commit_message>
rct upload today - john r.
</commit_message>
<xml_diff>
--- a/EXPORT.XLSX
+++ b/EXPORT.XLSX
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6602" uniqueCount="3186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6602" uniqueCount="3188">
   <si>
     <t>GNFXB</t>
   </si>
@@ -9022,6 +9022,9 @@
     <t>88473892</t>
   </si>
   <si>
+    <t>PM only arrrives mid Feb., therefore earlier start not possible, but FT set</t>
+  </si>
+  <si>
     <t>0000040582</t>
   </si>
   <si>
@@ -9546,6 +9549,9 @@
   </si>
   <si>
     <t>IXAROLA 10MG TAFI BLI 30 ZA</t>
+  </si>
+  <si>
+    <t>Start mid Feb. earliest possible, due to PM lead time // FT set, please also shorten transport time</t>
   </si>
   <si>
     <t>0000031666</t>
@@ -9783,28 +9789,28 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
-        <v>3178</v>
+        <v>3180</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>3179</v>
+        <v>3181</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>3180</v>
+        <v>3182</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3181</v>
+        <v>3183</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>3182</v>
+        <v>3184</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>3183</v>
+        <v>3185</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>3184</v>
+        <v>3186</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>3185</v>
+        <v>3187</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -24042,7 +24048,7 @@
         <v>1957</v>
       </c>
       <c r="H564" s="2">
-        <v>45278</v>
+        <v>45299</v>
       </c>
     </row>
     <row r="565" spans="1:8">
@@ -32039,31 +32045,33 @@
         <v>5</v>
       </c>
       <c r="G882" t="s">
-        <v>2</v>
-      </c>
-      <c r="H882" s="2"/>
+        <v>2974</v>
+      </c>
+      <c r="H882" s="2">
+        <v>45299</v>
+      </c>
     </row>
     <row r="883" spans="1:8">
       <c r="A883" t="s">
         <v>1562</v>
       </c>
       <c r="B883" t="s">
-        <v>2974</v>
+        <v>2975</v>
       </c>
       <c r="C883" t="s">
         <v>2926</v>
       </c>
       <c r="D883" t="s">
-        <v>2975</v>
+        <v>2976</v>
       </c>
       <c r="E883" t="s">
-        <v>2976</v>
+        <v>2977</v>
       </c>
       <c r="F883" t="s">
         <v>13</v>
       </c>
       <c r="G883" t="s">
-        <v>2977</v>
+        <v>2978</v>
       </c>
       <c r="H883" s="2">
         <v>45204</v>
@@ -32074,16 +32082,16 @@
         <v>1562</v>
       </c>
       <c r="B884" t="s">
-        <v>2978</v>
+        <v>2979</v>
       </c>
       <c r="C884" t="s">
         <v>2926</v>
       </c>
       <c r="D884" t="s">
-        <v>2979</v>
+        <v>2980</v>
       </c>
       <c r="E884" t="s">
-        <v>2980</v>
+        <v>2981</v>
       </c>
       <c r="F884" t="s">
         <v>5</v>
@@ -32098,22 +32106,22 @@
         <v>1562</v>
       </c>
       <c r="B885" t="s">
-        <v>2981</v>
+        <v>2982</v>
       </c>
       <c r="C885" t="s">
         <v>2926</v>
       </c>
       <c r="D885" t="s">
-        <v>2979</v>
+        <v>2980</v>
       </c>
       <c r="E885" t="s">
-        <v>2980</v>
+        <v>2981</v>
       </c>
       <c r="F885" t="s">
         <v>5</v>
       </c>
       <c r="G885" t="s">
-        <v>2982</v>
+        <v>2983</v>
       </c>
       <c r="H885" s="2">
         <v>45204</v>
@@ -32124,16 +32132,16 @@
         <v>1562</v>
       </c>
       <c r="B886" t="s">
-        <v>2983</v>
+        <v>2984</v>
       </c>
       <c r="C886" t="s">
         <v>2926</v>
       </c>
       <c r="D886" t="s">
-        <v>2984</v>
+        <v>2985</v>
       </c>
       <c r="E886" t="s">
-        <v>2985</v>
+        <v>2986</v>
       </c>
       <c r="F886" t="s">
         <v>5</v>
@@ -32148,16 +32156,16 @@
         <v>1344</v>
       </c>
       <c r="B887" t="s">
-        <v>2986</v>
+        <v>2987</v>
       </c>
       <c r="C887" t="s">
         <v>2926</v>
       </c>
       <c r="D887" t="s">
-        <v>2987</v>
+        <v>2988</v>
       </c>
       <c r="E887" t="s">
-        <v>2988</v>
+        <v>2989</v>
       </c>
       <c r="F887" t="s">
         <v>5</v>
@@ -32172,16 +32180,16 @@
         <v>1904</v>
       </c>
       <c r="B888" t="s">
-        <v>2989</v>
+        <v>2990</v>
       </c>
       <c r="C888" t="s">
         <v>2926</v>
       </c>
       <c r="D888" t="s">
-        <v>2990</v>
+        <v>2991</v>
       </c>
       <c r="E888" t="s">
-        <v>2991</v>
+        <v>2992</v>
       </c>
       <c r="F888" t="s">
         <v>18</v>
@@ -32193,25 +32201,25 @@
     </row>
     <row r="889" spans="1:8">
       <c r="A889" t="s">
-        <v>2992</v>
+        <v>2993</v>
       </c>
       <c r="B889" t="s">
-        <v>2993</v>
+        <v>2994</v>
       </c>
       <c r="C889" t="s">
-        <v>2994</v>
+        <v>2995</v>
       </c>
       <c r="D889" t="s">
-        <v>2995</v>
+        <v>2996</v>
       </c>
       <c r="E889" t="s">
-        <v>2996</v>
+        <v>2997</v>
       </c>
       <c r="F889" t="s">
         <v>69</v>
       </c>
       <c r="G889" t="s">
-        <v>2997</v>
+        <v>2998</v>
       </c>
       <c r="H889" s="2">
         <v>45278</v>
@@ -32222,16 +32230,16 @@
         <v>1463</v>
       </c>
       <c r="B890" t="s">
-        <v>2998</v>
+        <v>2999</v>
       </c>
       <c r="C890" t="s">
-        <v>2994</v>
+        <v>2995</v>
       </c>
       <c r="D890" t="s">
-        <v>2999</v>
+        <v>3000</v>
       </c>
       <c r="E890" t="s">
-        <v>3000</v>
+        <v>3001</v>
       </c>
       <c r="F890" t="s">
         <v>69</v>
@@ -32246,22 +32254,22 @@
         <v>469</v>
       </c>
       <c r="B891" t="s">
-        <v>3001</v>
+        <v>3002</v>
       </c>
       <c r="C891" t="s">
-        <v>2994</v>
+        <v>2995</v>
       </c>
       <c r="D891" t="s">
-        <v>3002</v>
+        <v>3003</v>
       </c>
       <c r="E891" t="s">
-        <v>3003</v>
+        <v>3004</v>
       </c>
       <c r="F891" t="s">
         <v>5</v>
       </c>
       <c r="G891" t="s">
-        <v>3004</v>
+        <v>3005</v>
       </c>
       <c r="H891" s="2">
         <v>45296</v>
@@ -32272,22 +32280,22 @@
         <v>469</v>
       </c>
       <c r="B892" t="s">
-        <v>3005</v>
+        <v>3006</v>
       </c>
       <c r="C892" t="s">
-        <v>2994</v>
+        <v>2995</v>
       </c>
       <c r="D892" t="s">
-        <v>3006</v>
+        <v>3007</v>
       </c>
       <c r="E892" t="s">
-        <v>3007</v>
+        <v>3008</v>
       </c>
       <c r="F892" t="s">
         <v>5</v>
       </c>
       <c r="G892" t="s">
-        <v>3008</v>
+        <v>3009</v>
       </c>
       <c r="H892" s="2">
         <v>45296</v>
@@ -32298,13 +32306,13 @@
         <v>2613</v>
       </c>
       <c r="B893" t="s">
-        <v>3009</v>
+        <v>3010</v>
       </c>
       <c r="C893" t="s">
-        <v>2994</v>
+        <v>2995</v>
       </c>
       <c r="D893" t="s">
-        <v>3010</v>
+        <v>3011</v>
       </c>
       <c r="E893" t="s">
         <v>1128</v>
@@ -32324,13 +32332,13 @@
         <v>469</v>
       </c>
       <c r="B894" t="s">
+        <v>3012</v>
+      </c>
+      <c r="C894" t="s">
+        <v>2995</v>
+      </c>
+      <c r="D894" t="s">
         <v>3011</v>
-      </c>
-      <c r="C894" t="s">
-        <v>2994</v>
-      </c>
-      <c r="D894" t="s">
-        <v>3010</v>
       </c>
       <c r="E894" t="s">
         <v>1128</v>
@@ -32339,7 +32347,7 @@
         <v>5</v>
       </c>
       <c r="G894" t="s">
-        <v>3012</v>
+        <v>3013</v>
       </c>
       <c r="H894" s="2">
         <v>45296</v>
@@ -32350,22 +32358,22 @@
         <v>469</v>
       </c>
       <c r="B895" t="s">
-        <v>3013</v>
+        <v>3014</v>
       </c>
       <c r="C895" t="s">
-        <v>2994</v>
+        <v>2995</v>
       </c>
       <c r="D895" t="s">
-        <v>3014</v>
+        <v>3015</v>
       </c>
       <c r="E895" t="s">
-        <v>3015</v>
+        <v>3016</v>
       </c>
       <c r="F895" t="s">
         <v>5</v>
       </c>
       <c r="G895" t="s">
-        <v>3016</v>
+        <v>3017</v>
       </c>
       <c r="H895" s="2">
         <v>45296</v>
@@ -32376,16 +32384,16 @@
         <v>2613</v>
       </c>
       <c r="B896" t="s">
-        <v>3017</v>
+        <v>3018</v>
       </c>
       <c r="C896" t="s">
-        <v>2994</v>
+        <v>2995</v>
       </c>
       <c r="D896" t="s">
-        <v>3018</v>
+        <v>3019</v>
       </c>
       <c r="E896" t="s">
-        <v>3019</v>
+        <v>3020</v>
       </c>
       <c r="F896" t="s">
         <v>5</v>
@@ -32402,16 +32410,16 @@
         <v>469</v>
       </c>
       <c r="B897" t="s">
-        <v>3020</v>
+        <v>3021</v>
       </c>
       <c r="C897" t="s">
-        <v>2994</v>
+        <v>2995</v>
       </c>
       <c r="D897" t="s">
-        <v>3021</v>
+        <v>3022</v>
       </c>
       <c r="E897" t="s">
-        <v>3022</v>
+        <v>3023</v>
       </c>
       <c r="F897" t="s">
         <v>13</v>
@@ -32428,22 +32436,22 @@
         <v>794</v>
       </c>
       <c r="B898" t="s">
-        <v>3023</v>
+        <v>3024</v>
       </c>
       <c r="C898" t="s">
-        <v>3024</v>
+        <v>3025</v>
       </c>
       <c r="D898" t="s">
-        <v>3025</v>
+        <v>3026</v>
       </c>
       <c r="E898" t="s">
-        <v>3026</v>
+        <v>3027</v>
       </c>
       <c r="F898" t="s">
         <v>13</v>
       </c>
       <c r="G898" t="s">
-        <v>3027</v>
+        <v>3028</v>
       </c>
       <c r="H898" s="2">
         <v>45295</v>
@@ -32454,22 +32462,22 @@
         <v>794</v>
       </c>
       <c r="B899" t="s">
-        <v>3028</v>
+        <v>3029</v>
       </c>
       <c r="C899" t="s">
-        <v>3024</v>
+        <v>3025</v>
       </c>
       <c r="D899" t="s">
-        <v>3029</v>
+        <v>3030</v>
       </c>
       <c r="E899" t="s">
-        <v>3030</v>
+        <v>3031</v>
       </c>
       <c r="F899" t="s">
         <v>13</v>
       </c>
       <c r="G899" t="s">
-        <v>3031</v>
+        <v>3032</v>
       </c>
       <c r="H899" s="2">
         <v>45296</v>
@@ -32480,16 +32488,16 @@
         <v>494</v>
       </c>
       <c r="B900" t="s">
-        <v>3032</v>
+        <v>3033</v>
       </c>
       <c r="C900" t="s">
-        <v>3024</v>
+        <v>3025</v>
       </c>
       <c r="D900" t="s">
-        <v>3033</v>
+        <v>3034</v>
       </c>
       <c r="E900" t="s">
-        <v>3034</v>
+        <v>3035</v>
       </c>
       <c r="F900" t="s">
         <v>13</v>
@@ -32504,22 +32512,22 @@
         <v>794</v>
       </c>
       <c r="B901" t="s">
-        <v>3035</v>
+        <v>3036</v>
       </c>
       <c r="C901" t="s">
-        <v>3024</v>
+        <v>3025</v>
       </c>
       <c r="D901" t="s">
-        <v>3036</v>
+        <v>3037</v>
       </c>
       <c r="E901" t="s">
-        <v>3037</v>
+        <v>3038</v>
       </c>
       <c r="F901" t="s">
         <v>5</v>
       </c>
       <c r="G901" t="s">
-        <v>3038</v>
+        <v>3039</v>
       </c>
       <c r="H901" s="2">
         <v>45295</v>
@@ -32530,22 +32538,22 @@
         <v>794</v>
       </c>
       <c r="B902" t="s">
-        <v>3039</v>
+        <v>3040</v>
       </c>
       <c r="C902" t="s">
-        <v>3024</v>
+        <v>3025</v>
       </c>
       <c r="D902" t="s">
-        <v>3036</v>
+        <v>3037</v>
       </c>
       <c r="E902" t="s">
-        <v>3037</v>
+        <v>3038</v>
       </c>
       <c r="F902" t="s">
         <v>5</v>
       </c>
       <c r="G902" t="s">
-        <v>3040</v>
+        <v>3041</v>
       </c>
       <c r="H902" s="2">
         <v>45267</v>
@@ -32556,16 +32564,16 @@
         <v>494</v>
       </c>
       <c r="B903" t="s">
-        <v>3041</v>
+        <v>3042</v>
       </c>
       <c r="C903" t="s">
-        <v>3024</v>
+        <v>3025</v>
       </c>
       <c r="D903" t="s">
-        <v>3042</v>
+        <v>3043</v>
       </c>
       <c r="E903" t="s">
-        <v>3043</v>
+        <v>3044</v>
       </c>
       <c r="F903" t="s">
         <v>5</v>
@@ -32580,22 +32588,22 @@
         <v>501</v>
       </c>
       <c r="B904" t="s">
-        <v>3044</v>
+        <v>3045</v>
       </c>
       <c r="C904" t="s">
-        <v>3024</v>
+        <v>3025</v>
       </c>
       <c r="D904" t="s">
-        <v>3045</v>
+        <v>3046</v>
       </c>
       <c r="E904" t="s">
-        <v>3046</v>
+        <v>3047</v>
       </c>
       <c r="F904" t="s">
         <v>5</v>
       </c>
       <c r="G904" t="s">
-        <v>3047</v>
+        <v>3048</v>
       </c>
       <c r="H904" s="2">
         <v>45246</v>
@@ -32603,19 +32611,19 @@
     </row>
     <row r="905" spans="1:8">
       <c r="A905" t="s">
-        <v>3048</v>
+        <v>3049</v>
       </c>
       <c r="B905" t="s">
-        <v>3049</v>
+        <v>3050</v>
       </c>
       <c r="C905" t="s">
-        <v>3024</v>
+        <v>3025</v>
       </c>
       <c r="D905" t="s">
-        <v>3050</v>
+        <v>3051</v>
       </c>
       <c r="E905" t="s">
-        <v>3051</v>
+        <v>3052</v>
       </c>
       <c r="F905" t="s">
         <v>5</v>
@@ -32627,19 +32635,19 @@
     </row>
     <row r="906" spans="1:8">
       <c r="A906" t="s">
-        <v>3048</v>
+        <v>3049</v>
       </c>
       <c r="B906" t="s">
-        <v>3052</v>
+        <v>3053</v>
       </c>
       <c r="C906" t="s">
-        <v>3024</v>
+        <v>3025</v>
       </c>
       <c r="D906" t="s">
-        <v>3053</v>
+        <v>3054</v>
       </c>
       <c r="E906" t="s">
-        <v>3054</v>
+        <v>3055</v>
       </c>
       <c r="F906" t="s">
         <v>877</v>
@@ -32651,25 +32659,25 @@
     </row>
     <row r="907" spans="1:8">
       <c r="A907" t="s">
-        <v>3048</v>
+        <v>3049</v>
       </c>
       <c r="B907" t="s">
-        <v>3055</v>
+        <v>3056</v>
       </c>
       <c r="C907" t="s">
-        <v>3024</v>
+        <v>3025</v>
       </c>
       <c r="D907" t="s">
-        <v>3056</v>
+        <v>3057</v>
       </c>
       <c r="E907" t="s">
-        <v>3057</v>
+        <v>3058</v>
       </c>
       <c r="F907" t="s">
         <v>877</v>
       </c>
       <c r="G907" t="s">
-        <v>3058</v>
+        <v>3059</v>
       </c>
       <c r="H907" s="2">
         <v>45265</v>
@@ -32677,19 +32685,19 @@
     </row>
     <row r="908" spans="1:8">
       <c r="A908" t="s">
-        <v>3048</v>
+        <v>3049</v>
       </c>
       <c r="B908" t="s">
-        <v>3059</v>
+        <v>3060</v>
       </c>
       <c r="C908" t="s">
-        <v>3024</v>
+        <v>3025</v>
       </c>
       <c r="D908" t="s">
-        <v>3060</v>
+        <v>3061</v>
       </c>
       <c r="E908" t="s">
-        <v>3061</v>
+        <v>3062</v>
       </c>
       <c r="F908" t="s">
         <v>877</v>
@@ -32701,19 +32709,19 @@
     </row>
     <row r="909" spans="1:8">
       <c r="A909" t="s">
-        <v>3048</v>
+        <v>3049</v>
       </c>
       <c r="B909" t="s">
-        <v>3062</v>
+        <v>3063</v>
       </c>
       <c r="C909" t="s">
-        <v>3024</v>
+        <v>3025</v>
       </c>
       <c r="D909" t="s">
-        <v>3063</v>
+        <v>3064</v>
       </c>
       <c r="E909" t="s">
-        <v>3064</v>
+        <v>3065</v>
       </c>
       <c r="F909" t="s">
         <v>877</v>
@@ -32728,16 +32736,16 @@
         <v>126</v>
       </c>
       <c r="B910" t="s">
-        <v>3065</v>
+        <v>3066</v>
       </c>
       <c r="C910" t="s">
-        <v>3024</v>
+        <v>3025</v>
       </c>
       <c r="D910" t="s">
-        <v>3066</v>
+        <v>3067</v>
       </c>
       <c r="E910" t="s">
-        <v>3067</v>
+        <v>3068</v>
       </c>
       <c r="F910" t="s">
         <v>18</v>
@@ -32752,16 +32760,16 @@
         <v>42</v>
       </c>
       <c r="B911" t="s">
-        <v>3068</v>
+        <v>3069</v>
       </c>
       <c r="C911" t="s">
-        <v>3069</v>
+        <v>3070</v>
       </c>
       <c r="D911" t="s">
-        <v>3070</v>
+        <v>3071</v>
       </c>
       <c r="E911" t="s">
-        <v>3071</v>
+        <v>3072</v>
       </c>
       <c r="F911" t="s">
         <v>5</v>
@@ -32776,13 +32784,13 @@
         <v>469</v>
       </c>
       <c r="B912" t="s">
-        <v>3072</v>
+        <v>3073</v>
       </c>
       <c r="C912" t="s">
-        <v>3073</v>
+        <v>3074</v>
       </c>
       <c r="D912" t="s">
-        <v>3074</v>
+        <v>3075</v>
       </c>
       <c r="E912" t="s">
         <v>2002</v>
@@ -32791,7 +32799,7 @@
         <v>69</v>
       </c>
       <c r="G912" t="s">
-        <v>3075</v>
+        <v>3076</v>
       </c>
       <c r="H912" s="2">
         <v>45296</v>
@@ -32802,13 +32810,13 @@
         <v>469</v>
       </c>
       <c r="B913" t="s">
-        <v>3076</v>
+        <v>3077</v>
       </c>
       <c r="C913" t="s">
-        <v>3073</v>
+        <v>3074</v>
       </c>
       <c r="D913" t="s">
-        <v>3077</v>
+        <v>3078</v>
       </c>
       <c r="E913" t="s">
         <v>389</v>
@@ -32817,7 +32825,7 @@
         <v>69</v>
       </c>
       <c r="G913" t="s">
-        <v>3078</v>
+        <v>3079</v>
       </c>
       <c r="H913" s="2">
         <v>45296</v>
@@ -32828,13 +32836,13 @@
         <v>1756</v>
       </c>
       <c r="B914" t="s">
-        <v>3079</v>
+        <v>3080</v>
       </c>
       <c r="C914" t="s">
-        <v>3080</v>
+        <v>3081</v>
       </c>
       <c r="D914" t="s">
-        <v>3081</v>
+        <v>3082</v>
       </c>
       <c r="E914" t="s">
         <v>927</v>
@@ -32852,16 +32860,16 @@
         <v>1904</v>
       </c>
       <c r="B915" t="s">
-        <v>3082</v>
+        <v>3083</v>
       </c>
       <c r="C915" t="s">
-        <v>3080</v>
+        <v>3081</v>
       </c>
       <c r="D915" t="s">
-        <v>3083</v>
+        <v>3084</v>
       </c>
       <c r="E915" t="s">
-        <v>3084</v>
+        <v>3085</v>
       </c>
       <c r="F915" t="s">
         <v>18</v>
@@ -32876,22 +32884,22 @@
         <v>1756</v>
       </c>
       <c r="B916" t="s">
-        <v>3085</v>
+        <v>3086</v>
       </c>
       <c r="C916" t="s">
-        <v>3080</v>
+        <v>3081</v>
       </c>
       <c r="D916" t="s">
-        <v>3086</v>
+        <v>3087</v>
       </c>
       <c r="E916" t="s">
-        <v>3087</v>
+        <v>3088</v>
       </c>
       <c r="F916" t="s">
         <v>18</v>
       </c>
       <c r="G916" t="s">
-        <v>3088</v>
+        <v>3089</v>
       </c>
       <c r="H916" s="2">
         <v>45278</v>
@@ -32902,16 +32910,16 @@
         <v>1562</v>
       </c>
       <c r="B917" t="s">
-        <v>3089</v>
+        <v>3090</v>
       </c>
       <c r="C917" t="s">
-        <v>3080</v>
+        <v>3081</v>
       </c>
       <c r="D917" t="s">
-        <v>3090</v>
+        <v>3091</v>
       </c>
       <c r="E917" t="s">
-        <v>3091</v>
+        <v>3092</v>
       </c>
       <c r="F917" t="s">
         <v>5</v>
@@ -32926,16 +32934,16 @@
         <v>1562</v>
       </c>
       <c r="B918" t="s">
-        <v>3092</v>
+        <v>3093</v>
       </c>
       <c r="C918" t="s">
-        <v>3080</v>
+        <v>3081</v>
       </c>
       <c r="D918" t="s">
-        <v>3093</v>
+        <v>3094</v>
       </c>
       <c r="E918" t="s">
-        <v>3094</v>
+        <v>3095</v>
       </c>
       <c r="F918" t="s">
         <v>5</v>
@@ -32950,22 +32958,22 @@
         <v>9</v>
       </c>
       <c r="B919" t="s">
-        <v>3095</v>
+        <v>3096</v>
       </c>
       <c r="C919" t="s">
-        <v>3096</v>
+        <v>3097</v>
       </c>
       <c r="D919" t="s">
-        <v>3097</v>
+        <v>3098</v>
       </c>
       <c r="E919" t="s">
-        <v>3098</v>
+        <v>3099</v>
       </c>
       <c r="F919" t="s">
         <v>5</v>
       </c>
       <c r="G919" t="s">
-        <v>3099</v>
+        <v>3100</v>
       </c>
       <c r="H919" s="2">
         <v>45239</v>
@@ -32976,16 +32984,16 @@
         <v>9</v>
       </c>
       <c r="B920" t="s">
-        <v>3100</v>
+        <v>3101</v>
       </c>
       <c r="C920" t="s">
-        <v>3096</v>
+        <v>3097</v>
       </c>
       <c r="D920" t="s">
-        <v>3101</v>
+        <v>3102</v>
       </c>
       <c r="E920" t="s">
-        <v>3102</v>
+        <v>3103</v>
       </c>
       <c r="F920" t="s">
         <v>5</v>
@@ -33000,16 +33008,16 @@
         <v>9</v>
       </c>
       <c r="B921" t="s">
-        <v>3103</v>
+        <v>3104</v>
       </c>
       <c r="C921" t="s">
-        <v>3096</v>
+        <v>3097</v>
       </c>
       <c r="D921" t="s">
-        <v>3104</v>
+        <v>3105</v>
       </c>
       <c r="E921" t="s">
-        <v>3105</v>
+        <v>3106</v>
       </c>
       <c r="F921" t="s">
         <v>69</v>
@@ -33024,16 +33032,16 @@
         <v>9</v>
       </c>
       <c r="B922" t="s">
-        <v>3106</v>
+        <v>3107</v>
       </c>
       <c r="C922" t="s">
-        <v>3096</v>
+        <v>3097</v>
       </c>
       <c r="D922" t="s">
-        <v>3107</v>
+        <v>3108</v>
       </c>
       <c r="E922" t="s">
-        <v>3108</v>
+        <v>3109</v>
       </c>
       <c r="F922" t="s">
         <v>5</v>
@@ -33048,16 +33056,16 @@
         <v>9</v>
       </c>
       <c r="B923" t="s">
-        <v>3109</v>
+        <v>3110</v>
       </c>
       <c r="C923" t="s">
-        <v>3096</v>
+        <v>3097</v>
       </c>
       <c r="D923" t="s">
-        <v>3110</v>
+        <v>3111</v>
       </c>
       <c r="E923" t="s">
-        <v>3111</v>
+        <v>3112</v>
       </c>
       <c r="F923" t="s">
         <v>5</v>
@@ -33072,16 +33080,16 @@
         <v>9</v>
       </c>
       <c r="B924" t="s">
-        <v>3112</v>
+        <v>3113</v>
       </c>
       <c r="C924" t="s">
-        <v>3096</v>
+        <v>3097</v>
       </c>
       <c r="D924" t="s">
-        <v>3113</v>
+        <v>3114</v>
       </c>
       <c r="E924" t="s">
-        <v>3114</v>
+        <v>3115</v>
       </c>
       <c r="F924" t="s">
         <v>5</v>
@@ -33096,16 +33104,16 @@
         <v>76</v>
       </c>
       <c r="B925" t="s">
-        <v>3115</v>
+        <v>3116</v>
       </c>
       <c r="C925" t="s">
-        <v>3096</v>
+        <v>3097</v>
       </c>
       <c r="D925" t="s">
-        <v>3116</v>
+        <v>3117</v>
       </c>
       <c r="E925" t="s">
-        <v>3117</v>
+        <v>3118</v>
       </c>
       <c r="F925" t="s">
         <v>5</v>
@@ -33122,22 +33130,22 @@
         <v>932</v>
       </c>
       <c r="B926" t="s">
-        <v>3118</v>
+        <v>3119</v>
       </c>
       <c r="C926" t="s">
-        <v>3096</v>
+        <v>3097</v>
       </c>
       <c r="D926" t="s">
-        <v>3119</v>
+        <v>3120</v>
       </c>
       <c r="E926" t="s">
-        <v>3120</v>
+        <v>3121</v>
       </c>
       <c r="F926" t="s">
         <v>5</v>
       </c>
       <c r="G926" t="s">
-        <v>3121</v>
+        <v>3122</v>
       </c>
       <c r="H926" s="2">
         <v>45279</v>
@@ -33148,13 +33156,13 @@
         <v>936</v>
       </c>
       <c r="B927" t="s">
-        <v>3122</v>
+        <v>3123</v>
       </c>
       <c r="C927" t="s">
-        <v>3096</v>
+        <v>3097</v>
       </c>
       <c r="D927" t="s">
-        <v>3123</v>
+        <v>3124</v>
       </c>
       <c r="E927" t="s">
         <v>935</v>
@@ -33172,22 +33180,22 @@
         <v>932</v>
       </c>
       <c r="B928" t="s">
-        <v>3124</v>
+        <v>3125</v>
       </c>
       <c r="C928" t="s">
-        <v>3096</v>
+        <v>3097</v>
       </c>
       <c r="D928" t="s">
-        <v>3125</v>
+        <v>3126</v>
       </c>
       <c r="E928" t="s">
-        <v>3126</v>
+        <v>3127</v>
       </c>
       <c r="F928" t="s">
         <v>5</v>
       </c>
       <c r="G928" t="s">
-        <v>3127</v>
+        <v>3128</v>
       </c>
       <c r="H928" s="2">
         <v>45229</v>
@@ -33198,22 +33206,22 @@
         <v>932</v>
       </c>
       <c r="B929" t="s">
-        <v>3128</v>
+        <v>3129</v>
       </c>
       <c r="C929" t="s">
-        <v>3096</v>
+        <v>3097</v>
       </c>
       <c r="D929" t="s">
-        <v>3125</v>
+        <v>3126</v>
       </c>
       <c r="E929" t="s">
-        <v>3126</v>
+        <v>3127</v>
       </c>
       <c r="F929" t="s">
         <v>5</v>
       </c>
       <c r="G929" t="s">
-        <v>3129</v>
+        <v>3130</v>
       </c>
       <c r="H929" s="2">
         <v>45258</v>
@@ -33224,22 +33232,22 @@
         <v>932</v>
       </c>
       <c r="B930" t="s">
-        <v>3130</v>
+        <v>3131</v>
       </c>
       <c r="C930" t="s">
-        <v>3096</v>
+        <v>3097</v>
       </c>
       <c r="D930" t="s">
-        <v>3125</v>
+        <v>3126</v>
       </c>
       <c r="E930" t="s">
-        <v>3126</v>
+        <v>3127</v>
       </c>
       <c r="F930" t="s">
         <v>5</v>
       </c>
       <c r="G930" t="s">
-        <v>3131</v>
+        <v>3132</v>
       </c>
       <c r="H930" s="2">
         <v>45239</v>
@@ -33250,22 +33258,22 @@
         <v>932</v>
       </c>
       <c r="B931" t="s">
+        <v>3133</v>
+      </c>
+      <c r="C931" t="s">
+        <v>3097</v>
+      </c>
+      <c r="D931" t="s">
+        <v>3126</v>
+      </c>
+      <c r="E931" t="s">
+        <v>3127</v>
+      </c>
+      <c r="F931" t="s">
+        <v>5</v>
+      </c>
+      <c r="G931" t="s">
         <v>3132</v>
-      </c>
-      <c r="C931" t="s">
-        <v>3096</v>
-      </c>
-      <c r="D931" t="s">
-        <v>3125</v>
-      </c>
-      <c r="E931" t="s">
-        <v>3126</v>
-      </c>
-      <c r="F931" t="s">
-        <v>5</v>
-      </c>
-      <c r="G931" t="s">
-        <v>3131</v>
       </c>
       <c r="H931" s="2">
         <v>45239</v>
@@ -33276,22 +33284,22 @@
         <v>936</v>
       </c>
       <c r="B932" t="s">
-        <v>3133</v>
+        <v>3134</v>
       </c>
       <c r="C932" t="s">
-        <v>3096</v>
+        <v>3097</v>
       </c>
       <c r="D932" t="s">
-        <v>3134</v>
+        <v>3135</v>
       </c>
       <c r="E932" t="s">
-        <v>3135</v>
+        <v>3136</v>
       </c>
       <c r="F932" t="s">
         <v>5</v>
       </c>
       <c r="G932" t="s">
-        <v>3136</v>
+        <v>3137</v>
       </c>
       <c r="H932" s="2">
         <v>45279</v>
@@ -33302,16 +33310,16 @@
         <v>936</v>
       </c>
       <c r="B933" t="s">
-        <v>3137</v>
+        <v>3138</v>
       </c>
       <c r="C933" t="s">
-        <v>3096</v>
+        <v>3097</v>
       </c>
       <c r="D933" t="s">
-        <v>3138</v>
+        <v>3139</v>
       </c>
       <c r="E933" t="s">
-        <v>3139</v>
+        <v>3140</v>
       </c>
       <c r="F933" t="s">
         <v>5</v>
@@ -33326,22 +33334,22 @@
         <v>936</v>
       </c>
       <c r="B934" t="s">
-        <v>3140</v>
+        <v>3141</v>
       </c>
       <c r="C934" t="s">
-        <v>3096</v>
+        <v>3097</v>
       </c>
       <c r="D934" t="s">
-        <v>3141</v>
+        <v>3142</v>
       </c>
       <c r="E934" t="s">
-        <v>3142</v>
+        <v>3143</v>
       </c>
       <c r="F934" t="s">
         <v>5</v>
       </c>
       <c r="G934" t="s">
-        <v>3143</v>
+        <v>3144</v>
       </c>
       <c r="H934" s="2">
         <v>45279</v>
@@ -33352,46 +33360,48 @@
         <v>936</v>
       </c>
       <c r="B935" t="s">
-        <v>3144</v>
+        <v>3145</v>
       </c>
       <c r="C935" t="s">
-        <v>3096</v>
+        <v>3097</v>
       </c>
       <c r="D935" t="s">
-        <v>3145</v>
+        <v>3146</v>
       </c>
       <c r="E935" t="s">
-        <v>3146</v>
+        <v>3147</v>
       </c>
       <c r="F935" t="s">
         <v>5</v>
       </c>
       <c r="G935" t="s">
-        <v>2</v>
-      </c>
-      <c r="H935" s="2"/>
+        <v>3148</v>
+      </c>
+      <c r="H935" s="2">
+        <v>45299</v>
+      </c>
     </row>
     <row r="936" spans="1:8">
       <c r="A936" t="s">
         <v>2262</v>
       </c>
       <c r="B936" t="s">
-        <v>3147</v>
+        <v>3149</v>
       </c>
       <c r="C936" t="s">
-        <v>3096</v>
+        <v>3097</v>
       </c>
       <c r="D936" t="s">
-        <v>3148</v>
+        <v>3150</v>
       </c>
       <c r="E936" t="s">
-        <v>3149</v>
+        <v>3151</v>
       </c>
       <c r="F936" t="s">
         <v>69</v>
       </c>
       <c r="G936" t="s">
-        <v>3150</v>
+        <v>3152</v>
       </c>
       <c r="H936" s="2">
         <v>45113</v>
@@ -33402,22 +33412,22 @@
         <v>9</v>
       </c>
       <c r="B937" t="s">
-        <v>3151</v>
+        <v>3153</v>
       </c>
       <c r="C937" t="s">
-        <v>3096</v>
+        <v>3097</v>
       </c>
       <c r="D937" t="s">
-        <v>3152</v>
+        <v>3154</v>
       </c>
       <c r="E937" t="s">
-        <v>3153</v>
+        <v>3155</v>
       </c>
       <c r="F937" t="s">
         <v>69</v>
       </c>
       <c r="G937" t="s">
-        <v>3154</v>
+        <v>3156</v>
       </c>
       <c r="H937" s="2">
         <v>45113</v>
@@ -33428,22 +33438,22 @@
         <v>505</v>
       </c>
       <c r="B938" t="s">
-        <v>3155</v>
+        <v>3157</v>
       </c>
       <c r="C938" t="s">
-        <v>3096</v>
+        <v>3097</v>
       </c>
       <c r="D938" t="s">
-        <v>3156</v>
+        <v>3158</v>
       </c>
       <c r="E938" t="s">
-        <v>3157</v>
+        <v>3159</v>
       </c>
       <c r="F938" t="s">
         <v>5</v>
       </c>
       <c r="G938" t="s">
-        <v>3158</v>
+        <v>3160</v>
       </c>
       <c r="H938" s="2">
         <v>45296</v>
@@ -33454,22 +33464,22 @@
         <v>9</v>
       </c>
       <c r="B939" t="s">
-        <v>3159</v>
+        <v>3161</v>
       </c>
       <c r="C939" t="s">
-        <v>3096</v>
+        <v>3097</v>
       </c>
       <c r="D939" t="s">
-        <v>3160</v>
+        <v>3162</v>
       </c>
       <c r="E939" t="s">
-        <v>3161</v>
+        <v>3163</v>
       </c>
       <c r="F939" t="s">
         <v>5</v>
       </c>
       <c r="G939" t="s">
-        <v>3162</v>
+        <v>3164</v>
       </c>
       <c r="H939" s="2">
         <v>45202</v>
@@ -33480,22 +33490,22 @@
         <v>9</v>
       </c>
       <c r="B940" t="s">
-        <v>3163</v>
+        <v>3165</v>
       </c>
       <c r="C940" t="s">
-        <v>3096</v>
+        <v>3097</v>
       </c>
       <c r="D940" t="s">
-        <v>3164</v>
+        <v>3166</v>
       </c>
       <c r="E940" t="s">
-        <v>3165</v>
+        <v>3167</v>
       </c>
       <c r="F940" t="s">
         <v>69</v>
       </c>
       <c r="G940" t="s">
-        <v>3166</v>
+        <v>3168</v>
       </c>
       <c r="H940" s="2">
         <v>45215</v>
@@ -33506,22 +33516,22 @@
         <v>9</v>
       </c>
       <c r="B941" t="s">
-        <v>3167</v>
+        <v>3169</v>
       </c>
       <c r="C941" t="s">
-        <v>3096</v>
+        <v>3097</v>
       </c>
       <c r="D941" t="s">
-        <v>3168</v>
+        <v>3170</v>
       </c>
       <c r="E941" t="s">
-        <v>3169</v>
+        <v>3171</v>
       </c>
       <c r="F941" t="s">
         <v>69</v>
       </c>
       <c r="G941" t="s">
-        <v>3170</v>
+        <v>3172</v>
       </c>
       <c r="H941" s="2">
         <v>45215</v>
@@ -33532,22 +33542,22 @@
         <v>76</v>
       </c>
       <c r="B942" t="s">
-        <v>3171</v>
+        <v>3173</v>
       </c>
       <c r="C942" t="s">
-        <v>3096</v>
+        <v>3097</v>
       </c>
       <c r="D942" t="s">
-        <v>3172</v>
+        <v>3174</v>
       </c>
       <c r="E942" t="s">
-        <v>3173</v>
+        <v>3175</v>
       </c>
       <c r="F942" t="s">
         <v>5</v>
       </c>
       <c r="G942" t="s">
-        <v>3174</v>
+        <v>3176</v>
       </c>
       <c r="H942" s="2">
         <v>45211</v>
@@ -33558,16 +33568,16 @@
         <v>505</v>
       </c>
       <c r="B943" t="s">
-        <v>3175</v>
+        <v>3177</v>
       </c>
       <c r="C943" t="s">
-        <v>3096</v>
+        <v>3097</v>
       </c>
       <c r="D943" t="s">
-        <v>3176</v>
+        <v>3178</v>
       </c>
       <c r="E943" t="s">
-        <v>3177</v>
+        <v>3179</v>
       </c>
       <c r="F943" t="s">
         <v>18</v>

</xml_diff>